<commit_message>
aussie open round 2 part 1
</commit_message>
<xml_diff>
--- a/Data/2019.xlsx
+++ b/Data/2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="234">
   <si>
     <t xml:space="preserve">ATP</t>
   </si>
@@ -673,7 +673,55 @@
     <t xml:space="preserve">Carreno Busta P.</t>
   </si>
   <si>
-    <t xml:space="preserve">De Minaur A.</t>
+    <t xml:space="preserve">Melbourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australian Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Slam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nadal R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federer R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cilic M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomic B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molleker R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipsarevic J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monfils G.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evans D.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ito T.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laaksonen H.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delbonis F.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez F.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travaglia S.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troicki V.</t>
   </si>
 </sst>
 </file>
@@ -794,34 +842,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN200"/>
+  <dimension ref="A1:AN232"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D164" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E191" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A164" activeCellId="0" sqref="A164"/>
-      <selection pane="bottomRight" activeCell="I180" activeCellId="0" sqref="I180"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A191" activeCellId="0" sqref="A191"/>
+      <selection pane="bottomRight" activeCell="J231" activeCellId="0" sqref="J231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.45408163265306"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.45408163265306"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.23979591836735"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="3.23979591836735"/>
@@ -832,17 +879,18 @@
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="3.23979591836735"/>
     <col collapsed="false" hidden="false" max="27" min="26" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="30" min="29" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="4.59183673469388"/>
     <col collapsed="false" hidden="false" max="40" min="39" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14702,7 +14750,7 @@
         <v>3</v>
       </c>
       <c r="J198" s="0" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
       <c r="K198" s="0" t="s">
         <v>114</v>
@@ -14875,6 +14923,2506 @@
       </c>
       <c r="AD200" s="0" t="n">
         <v>1.69</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D201" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E201" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F201" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G201" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H201" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I201" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J201" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="K201" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="L201" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M201" s="0" t="n">
+        <v>238</v>
+      </c>
+      <c r="P201" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q201" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R201" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S201" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T201" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U201" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z201" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB201" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC201" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="AD201" s="0" t="n">
+        <v>11.64</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D202" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E202" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F202" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G202" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H202" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I202" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J202" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="K202" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="L202" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M202" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="P202" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q202" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R202" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S202" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T202" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U202" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z202" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB202" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC202" s="0" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="AD202" s="0" t="n">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D203" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E203" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F203" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G203" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H203" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I203" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J203" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="K203" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="L203" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M203" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="P203" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q203" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R203" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="S203" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="T203" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U203" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V203" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W203" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z203" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA203" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB203" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC203" s="0" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="AD203" s="0" t="n">
+        <v>10.18</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C204" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D204" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E204" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F204" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G204" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H204" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I204" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J204" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="K204" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="L204" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M204" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="P204" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q204" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R204" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S204" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T204" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U204" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z204" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB204" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC204" s="0" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="AD204" s="0" t="n">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D205" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E205" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F205" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G205" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H205" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I205" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J205" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="K205" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="L205" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="M205" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="P205" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q205" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R205" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S205" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T205" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U205" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V205" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W205" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z205" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA205" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB205" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC205" s="0" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AD205" s="0" t="n">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D206" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E206" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F206" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G206" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H206" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I206" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J206" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="K206" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="L206" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M206" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="P206" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q206" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R206" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S206" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T206" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U206" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V206" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W206" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z206" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA206" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB206" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC206" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AD206" s="0" t="n">
+        <v>7.31</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D207" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E207" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F207" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G207" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H207" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I207" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J207" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K207" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="L207" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="M207" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P207" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q207" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R207" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T207" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U207" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z207" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB207" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC207" s="0" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AD207" s="0" t="n">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D208" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E208" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F208" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G208" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H208" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I208" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J208" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="K208" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="L208" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M208" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="P208" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q208" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R208" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S208" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T208" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U208" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V208" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W208" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z208" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA208" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB208" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC208" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AD208" s="0" t="n">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D209" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E209" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F209" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G209" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H209" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I209" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J209" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="K209" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="L209" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="M209" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="P209" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q209" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R209" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S209" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T209" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U209" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V209" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z209" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA209" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB209" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC209" s="0" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="AD209" s="0" t="n">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D210" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E210" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F210" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G210" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H210" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I210" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J210" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="K210" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="L210" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M210" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="P210" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q210" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R210" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S210" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T210" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U210" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V210" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W210" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z210" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA210" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB210" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC210" s="0" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="AD210" s="0" t="n">
+        <v>4.36</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C211" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D211" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E211" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F211" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G211" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H211" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I211" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J211" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="K211" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="L211" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M211" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="P211" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q211" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R211" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S211" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T211" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U211" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V211" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W211" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z211" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA211" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB211" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC211" s="0" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="AD211" s="0" t="n">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D212" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E212" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G212" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H212" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I212" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J212" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="K212" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="L212" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="M212" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="P212" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q212" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R212" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S212" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T212" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U212" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V212" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W212" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="X212" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y212" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z212" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA212" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB212" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC212" s="0" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="AD212" s="0" t="n">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D213" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E213" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F213" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G213" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H213" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I213" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J213" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="K213" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="L213" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="M213" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="P213" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q213" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R213" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S213" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T213" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U213" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z213" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB213" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC213" s="0" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="AD213" s="0" t="n">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D214" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E214" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F214" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G214" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H214" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I214" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J214" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="K214" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="L214" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="M214" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="P214" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q214" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R214" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S214" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T214" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U214" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z214" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB214" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC214" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="AD214" s="0" t="n">
+        <v>11.61</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D215" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E215" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F215" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G215" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H215" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I215" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J215" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="K215" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="L215" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="M215" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="P215" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R215" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S215" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T215" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z215" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB215" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC215" s="0" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="AD215" s="0" t="n">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D216" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E216" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F216" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G216" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H216" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I216" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J216" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K216" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="L216" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="M216" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="P216" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q216" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R216" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S216" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T216" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U216" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V216" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W216" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z216" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA216" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB216" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC216" s="0" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="AD216" s="0" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D217" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E217" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F217" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G217" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H217" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I217" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J217" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="K217" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="L217" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="M217" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="P217" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q217" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R217" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S217" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T217" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U217" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V217" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W217" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z217" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA217" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB217" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC217" s="0" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="AD217" s="0" t="n">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D218" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E218" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F218" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G218" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H218" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I218" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J218" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="K218" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="L218" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="M218" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="P218" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q218" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R218" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S218" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T218" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U218" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z218" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA218" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB218" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC218" s="0" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="AD218" s="0" t="n">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D219" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E219" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F219" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G219" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H219" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I219" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J219" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="K219" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="L219" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="M219" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="P219" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q219" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R219" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S219" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T219" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U219" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V219" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W219" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z219" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA219" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB219" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC219" s="0" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="AD219" s="0" t="n">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C220" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D220" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E220" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F220" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G220" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H220" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I220" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J220" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="K220" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="L220" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="M220" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="P220" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q220" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R220" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S220" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T220" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U220" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z220" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA220" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB220" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC220" s="0" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="AD220" s="0" t="n">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C221" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D221" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E221" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F221" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G221" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H221" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I221" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J221" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="K221" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="L221" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M221" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="P221" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q221" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R221" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S221" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T221" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U221" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V221" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W221" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z221" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA221" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB221" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC221" s="0" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="AD221" s="0" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D222" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E222" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F222" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G222" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H222" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I222" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J222" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="K222" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="L222" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="M222" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="P222" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q222" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R222" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S222" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T222" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U222" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z222" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA222" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB222" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC222" s="0" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="AD222" s="0" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D223" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E223" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F223" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G223" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H223" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I223" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J223" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K223" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L223" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="M223" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="P223" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q223" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R223" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S223" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T223" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U223" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z223" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA223" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB223" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC223" s="0" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="AD223" s="0" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C224" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D224" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E224" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F224" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G224" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H224" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I224" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J224" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="K224" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="L224" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="M224" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="P224" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q224" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R224" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S224" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T224" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U224" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V224" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W224" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="X224" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y224" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z224" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA224" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB224" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC224" s="0" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="AD224" s="0" t="n">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C225" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D225" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E225" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F225" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G225" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H225" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I225" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J225" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="K225" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="L225" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="M225" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="P225" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q225" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R225" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S225" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T225" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U225" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V225" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W225" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z225" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA225" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB225" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC225" s="0" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="AD225" s="0" t="n">
+        <v>2.03</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D226" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E226" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F226" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G226" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H226" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I226" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J226" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="K226" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="L226" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="M226" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="P226" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q226" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R226" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S226" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T226" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U226" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V226" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W226" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z226" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA226" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB226" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC226" s="0" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="AD226" s="0" t="n">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D227" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E227" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F227" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G227" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H227" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I227" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J227" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="K227" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="L227" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="M227" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="P227" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q227" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R227" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S227" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T227" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U227" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V227" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W227" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z227" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA227" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB227" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC227" s="0" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="AD227" s="0" t="n">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D228" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E228" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F228" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G228" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H228" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I228" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J228" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="K228" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="L228" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="M228" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="P228" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q228" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R228" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S228" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T228" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U228" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V228" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W228" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z228" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA228" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB228" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC228" s="0" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="AD228" s="0" t="n">
+        <v>2.07</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B229" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C229" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D229" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E229" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F229" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G229" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H229" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I229" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J229" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="K229" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="L229" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="M229" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="P229" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q229" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R229" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S229" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T229" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U229" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z229" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA229" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB229" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC229" s="0" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="AD229" s="0" t="n">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C230" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D230" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E230" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F230" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G230" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H230" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I230" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J230" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="K230" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="L230" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="M230" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="P230" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q230" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R230" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S230" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T230" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U230" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z230" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB230" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC230" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AD230" s="0" t="n">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C231" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D231" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E231" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F231" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G231" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H231" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I231" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J231" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="K231" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="L231" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="M231" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="P231" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q231" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R231" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S231" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T231" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U231" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V231" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W231" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z231" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA231" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB231" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC231" s="0" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="AD231" s="0" t="n">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B232" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C232" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D232" s="1" t="n">
+        <v>43479</v>
+      </c>
+      <c r="E232" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F232" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G232" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H232" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I232" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J232" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="K232" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="L232" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="M232" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="P232" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q232" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R232" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S232" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T232" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U232" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V232" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W232" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X232" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y232" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z232" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA232" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB232" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC232" s="0" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="AD232" s="0" t="n">
+        <v>3.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data prep for 17th jan
</commit_message>
<xml_diff>
--- a/Data/2019.xlsx
+++ b/Data/2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="246">
   <si>
     <t xml:space="preserve">ATP</t>
   </si>
@@ -722,6 +722,42 @@
   </si>
   <si>
     <t xml:space="preserve">Troicki V.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krueger M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zverev A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Majchrzak K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coric B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harris L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krajinovic F.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanni L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kukushkin M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li Z.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sock J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakharov G.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zverev M.</t>
   </si>
 </sst>
 </file>
@@ -842,33 +878,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN232"/>
+  <dimension ref="A1:AN264"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I221" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A191" activeCellId="0" sqref="A191"/>
-      <selection pane="bottomRight" activeCell="J231" activeCellId="0" sqref="J231"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A221" activeCellId="0" sqref="A221"/>
+      <selection pane="bottomRight" activeCell="J264" activeCellId="0" sqref="J264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.32142857142857"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.32142857142857"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.23979591836735"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="3.23979591836735"/>
@@ -879,18 +915,17 @@
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="3.23979591836735"/>
     <col collapsed="false" hidden="false" max="27" min="26" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="30" min="29" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="4.45408163265306"/>
     <col collapsed="false" hidden="false" max="40" min="39" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17423,6 +17458,2476 @@
       </c>
       <c r="AD232" s="0" t="n">
         <v>3.35</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D233" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E233" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F233" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G233" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H233" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I233" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J233" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="K233" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="L233" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M233" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="P233" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q233" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R233" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S233" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T233" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U233" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z233" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB233" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC233" s="0" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="AD233" s="0" t="n">
+        <v>23.37</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C234" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D234" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E234" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F234" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G234" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H234" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I234" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J234" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="K234" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="L234" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="M234" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="P234" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q234" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R234" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S234" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T234" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U234" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z234" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB234" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC234" s="0" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="AD234" s="0" t="n">
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C235" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D235" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E235" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F235" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G235" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H235" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I235" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J235" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="K235" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="L235" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="M235" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="P235" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q235" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R235" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S235" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T235" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U235" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V235" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W235" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X235" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y235" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z235" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA235" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB235" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC235" s="0" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="AD235" s="0" t="n">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C236" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D236" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E236" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F236" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G236" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H236" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I236" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J236" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="K236" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="L236" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="M236" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="P236" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q236" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R236" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S236" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="T236" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V236" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W236" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X236" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z236" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA236" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB236" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC236" s="0" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="AD236" s="0" t="n">
+        <v>16.14</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D237" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E237" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F237" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G237" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H237" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I237" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J237" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="K237" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L237" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M237" s="0" t="n">
+        <v>321</v>
+      </c>
+      <c r="P237" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q237" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R237" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S237" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T237" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U237" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z237" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB237" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC237" s="0" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="AD237" s="0" t="n">
+        <v>5.42</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D238" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E238" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F238" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G238" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H238" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I238" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J238" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="K238" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="L238" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M238" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="P238" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q238" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R238" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S238" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T238" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U238" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z238" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB238" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC238" s="0" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="AD238" s="0" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C239" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D239" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E239" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F239" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G239" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H239" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I239" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J239" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="K239" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="L239" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="M239" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="P239" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q239" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R239" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S239" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T239" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U239" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z239" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB239" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC239" s="0" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="AD239" s="0" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B240" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C240" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D240" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E240" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F240" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G240" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H240" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I240" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J240" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K240" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="L240" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M240" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="P240" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q240" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R240" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S240" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T240" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U240" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z240" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB240" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC240" s="0" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="AD240" s="0" t="n">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C241" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D241" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E241" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F241" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G241" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H241" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I241" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J241" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="K241" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="L241" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="M241" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="P241" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q241" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S241" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T241" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U241" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V241" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W241" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X241" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y241" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z241" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA241" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB241" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC241" s="0" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="AD241" s="0" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C242" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D242" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E242" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F242" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G242" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H242" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I242" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J242" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="K242" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="L242" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M242" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="P242" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R242" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S242" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T242" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U242" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z242" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB242" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC242" s="0" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="AD242" s="0" t="n">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D243" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E243" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F243" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G243" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H243" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I243" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J243" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="K243" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="L243" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="M243" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="P243" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q243" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R243" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S243" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T243" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U243" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V243" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W243" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="X243" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y243" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z243" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA243" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB243" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC243" s="0" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="AD243" s="0" t="n">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B244" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C244" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D244" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E244" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F244" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G244" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H244" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I244" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J244" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="K244" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="L244" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="M244" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="P244" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q244" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R244" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S244" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="T244" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U244" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V244" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W244" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X244" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y244" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z244" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA244" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB244" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC244" s="0" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="AD244" s="0" t="n">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B245" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D245" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E245" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F245" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G245" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H245" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I245" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J245" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="K245" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="L245" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="M245" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="P245" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q245" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R245" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S245" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T245" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U245" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z245" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB245" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D246" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E246" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F246" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G246" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H246" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I246" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J246" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="K246" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="L246" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="M246" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="P246" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q246" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R246" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S246" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T246" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U246" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z246" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB246" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC246" s="0" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="AD246" s="0" t="n">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D247" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E247" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F247" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G247" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H247" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I247" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J247" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="K247" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L247" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M247" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="P247" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q247" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R247" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S247" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T247" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U247" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z247" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB247" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC247" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AD247" s="0" t="n">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B248" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D248" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E248" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F248" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G248" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H248" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I248" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J248" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="K248" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="L248" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="M248" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="P248" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q248" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R248" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S248" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T248" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U248" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z248" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA248" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB248" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC248" s="0" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="AD248" s="0" t="n">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B249" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D249" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E249" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F249" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G249" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H249" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I249" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J249" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="K249" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="L249" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="M249" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="P249" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q249" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R249" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S249" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T249" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U249" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V249" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W249" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z249" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA249" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB249" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC249" s="0" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="AD249" s="0" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B250" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D250" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E250" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F250" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G250" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H250" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I250" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J250" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="K250" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="L250" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="M250" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="P250" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q250" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R250" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S250" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T250" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U250" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V250" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W250" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="X250" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y250" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z250" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA250" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB250" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC250" s="0" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="AD250" s="0" t="n">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D251" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E251" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F251" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G251" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H251" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I251" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J251" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K251" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L251" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M251" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="P251" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q251" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R251" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S251" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T251" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U251" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z251" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB251" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC251" s="0" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="AD251" s="0" t="n">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C252" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D252" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E252" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F252" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G252" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H252" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I252" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J252" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K252" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L252" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="M252" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="P252" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q252" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R252" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S252" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z252" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA252" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB252" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC252" s="0" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="AD252" s="0" t="n">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B253" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C253" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D253" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E253" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F253" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G253" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H253" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I253" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J253" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K253" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="L253" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="M253" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="P253" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q253" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R253" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S253" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T253" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U253" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V253" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W253" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z253" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA253" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB253" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC253" s="0" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="AD253" s="0" t="n">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B254" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C254" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D254" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E254" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F254" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G254" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H254" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I254" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J254" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="K254" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="L254" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="M254" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="P254" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q254" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R254" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S254" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T254" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U254" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V254" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W254" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z254" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA254" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB254" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B255" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C255" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D255" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E255" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F255" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G255" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H255" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I255" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J255" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="K255" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="L255" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="M255" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="P255" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q255" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R255" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S255" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T255" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U255" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z255" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA255" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB255" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC255" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AD255" s="0" t="n">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B256" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C256" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D256" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E256" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F256" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G256" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H256" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I256" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J256" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K256" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="L256" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="M256" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="P256" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q256" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R256" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S256" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T256" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U256" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V256" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W256" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z256" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA256" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB256" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC256" s="0" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AD256" s="0" t="n">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B257" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C257" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D257" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E257" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F257" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G257" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H257" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I257" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J257" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="K257" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="L257" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="M257" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="P257" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q257" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R257" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S257" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T257" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U257" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V257" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W257" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z257" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA257" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB257" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC257" s="0" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="AD257" s="0" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B258" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C258" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D258" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E258" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F258" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G258" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H258" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I258" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J258" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="K258" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="L258" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="M258" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="P258" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q258" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R258" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S258" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T258" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U258" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V258" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W258" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z258" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA258" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB258" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC258" s="0" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="AD258" s="0" t="n">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B259" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C259" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D259" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E259" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F259" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G259" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H259" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I259" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J259" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K259" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="L259" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="M259" s="0" t="n">
+        <v>252</v>
+      </c>
+      <c r="P259" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q259" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R259" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S259" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T259" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U259" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z259" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA259" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB259" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC259" s="0" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="AD259" s="0" t="n">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B260" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C260" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D260" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E260" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F260" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G260" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H260" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I260" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J260" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K260" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="L260" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="M260" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="P260" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q260" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R260" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S260" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T260" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U260" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V260" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W260" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z260" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA260" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB260" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC260" s="0" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="AD260" s="0" t="n">
+        <v>2.03</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B261" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C261" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D261" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E261" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F261" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G261" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H261" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I261" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J261" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="K261" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="L261" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="M261" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="P261" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q261" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R261" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S261" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T261" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U261" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z261" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA261" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB261" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC261" s="0" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="AD261" s="0" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D262" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E262" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F262" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G262" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H262" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I262" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J262" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="K262" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="L262" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="M262" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="P262" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q262" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R262" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S262" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T262" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U262" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V262" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W262" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X262" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y262" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z262" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA262" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB262" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC262" s="0" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="AD262" s="0" t="n">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D263" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E263" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F263" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G263" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H263" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I263" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J263" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="K263" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="L263" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="M263" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="P263" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q263" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R263" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S263" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T263" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U263" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z263" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA263" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB263" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC263" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AD263" s="0" t="n">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C264" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D264" s="1" t="n">
+        <v>43480</v>
+      </c>
+      <c r="E264" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F264" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G264" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H264" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I264" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J264" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="K264" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="L264" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="M264" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="P264" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q264" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R264" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S264" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z264" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA264" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB264" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC264" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AD264" s="0" t="n">
+        <v>4.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>